<commit_message>
283 préparation de la release 110 (#290)
* release110

* Update release-notes.md

* prepublication b441dca0c64ab6de8fea56f161ebcba441658b41
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tddui-bundle.xlsx
+++ b/main/ig/StructureDefinition-tddui-bundle.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0-ballot</t>
+    <t>1.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-02-24T10:50:39+00:00</t>
+    <t>2025-02-24T14:10:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Mise à jour de la dépendance avec l'IG terminonogies (#323)
* maj dépendance IG termino

* Update sushi-config.yaml be03cb7ab146bd9efad8e584a7414beaf853cafc
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tddui-bundle.xlsx
+++ b/main/ig/StructureDefinition-tddui-bundle.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-25T10:12:59+00:00</t>
+    <t>2025-07-08T07:51:56+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1306,17 +1306,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="61.7734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="39.0078125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="23.19140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="21.21875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9453125" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.4296875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="52.95703125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="19.8828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="18.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="103.296875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="88.55859375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1325,26 +1325,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="9.953125" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="18.859375" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="168.19140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="49.01171875" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="22.71875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="50.03125" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.98046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="10.5546875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="11.0390625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="144.1953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="42.89453125" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="28.1484375" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="50.08203125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="42.9765625" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="36.91796875" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="24.1328125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="42.9375" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
ANS-006-150 - Restructuration du guide d'implémentation (#327)
* SuppressionCDA_RestructurationIG

* ongletRC

* indexSuppressionCDA

* RestructurationIG_reviewJGT

* RestructurationIG_MAJSommaire

* RestructurationIG_AjoutAnnexePageAccueil

* RestructurationIG_AjoutAnnexePS-correctionQA eac7eb143002b324916f6357cb4ffd37a1b1b344
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tddui-bundle.xlsx
+++ b/main/ig/StructureDefinition-tddui-bundle.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2930" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="269">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-31T08:12:23+00:00</t>
+    <t>2025-07-31T08:39:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -576,16 +576,6 @@
     <t>An entry in a bundle resource - will either contain a resource or information about a resource (transactions and history only).</t>
   </si>
   <si>
-    <t xml:space="preserve">profile:resource}
-</t>
-  </si>
-  <si>
-    <t>Slicing based on the profile conformance of the entry</t>
-  </si>
-  <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>bdl-5:must be a resource unless there's a request or response {resource.exists() or request.exists() or response.exists()}
 bdl-8:fullUrl cannot be a version specific reference {fullUrl.contains('/_history/').not()}ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}</t>
   </si>
@@ -850,130 +840,6 @@
   <si>
     <t>For a POST/PUT operation, this is the equivalent outcome that would be returned for prefer = operationoutcome - except that the resource is always returned whether or not the outcome is returned.
 This outcome is not used for error responses in batch/transaction, only for hints and warnings. In a batch operation, the error will be in Bundle.entry.response, and for transaction, there will be a single OperationOutcome instead of a bundle in the case of an error.</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference</t>
-  </si>
-  <si>
-    <t>DUIDocumentReference</t>
-  </si>
-  <si>
-    <t>DocumentReference conforming to the TDDUIDocumentReference profile, used to convey a document in CDA format.</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.link</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.fullUrl</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.resource</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DocumentReference {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-documentreference}
-</t>
-  </si>
-  <si>
-    <t>A reference to a document</t>
-  </si>
-  <si>
-    <t>A reference to a document of any kind for any purpose. Provides metadata about the document so that the document can be discovered and managed. The scope of a document is any seralized object with a mime-type, so includes formal patient centric documents (CDA), cliical notes, scanned paper, and non-patient specific documents like policy text.</t>
-  </si>
-  <si>
-    <t>Usually, this is used for documents other than those defined by FHIR.</t>
-  </si>
-  <si>
-    <t>Document[classCode="DOC" and moodCode="EVN"]</t>
-  </si>
-  <si>
-    <t>when describing a CDA</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.search</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.search.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.search.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.search.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.search.mode</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.search.score</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.method</t>
-  </si>
-  <si>
-    <t>POST</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.url</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.ifNoneMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.ifModifiedSince</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.ifMatch</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.request.ifNoneExist</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.id</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.extension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.modifierExtension</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.status</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.location</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.etag</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.lastModified</t>
-  </si>
-  <si>
-    <t>Bundle.entry:DUIDocumentReference.response.outcome</t>
   </si>
   <si>
     <t>Bundle.signature</t>
@@ -1297,7 +1163,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN81"/>
+  <dimension ref="A1:AN49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1306,9 +1172,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="52.95703125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="33.44140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="19.8828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="10.8515625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="18.19140625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
@@ -1316,7 +1182,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="88.55859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="15.140625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1334,7 +1200,7 @@
     <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="42.89453125" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1342,7 +1208,7 @@
     <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
     <col min="37" max="37" width="24.1328125" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="42.9375" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="21.4140625" customWidth="true" bestFit="true"/>
     <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
@@ -3184,7 +3050,7 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>79</v>
@@ -3244,16 +3110,16 @@
         <v>77</v>
       </c>
       <c r="AB17" t="s" s="2">
-        <v>178</v>
+        <v>77</v>
       </c>
       <c r="AC17" t="s" s="2">
-        <v>179</v>
+        <v>77</v>
       </c>
       <c r="AD17" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>180</v>
+        <v>77</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>175</v>
@@ -3268,7 +3134,7 @@
         <v>77</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>77</v>
@@ -3285,10 +3151,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -3397,10 +3263,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -3511,10 +3377,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -3627,10 +3493,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -3656,10 +3522,10 @@
         <v>80</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -3710,7 +3576,7 @@
         <v>77</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>78</v>
@@ -3739,10 +3605,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3768,13 +3634,13 @@
         <v>101</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="N22" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" t="s" s="2">
@@ -3824,7 +3690,7 @@
         <v>77</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>78</v>
@@ -3853,10 +3719,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -3879,13 +3745,13 @@
         <v>88</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -3936,7 +3802,7 @@
         <v>77</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>78</v>
@@ -3965,10 +3831,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3994,10 +3860,10 @@
         <v>145</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -4048,16 +3914,16 @@
         <v>77</v>
       </c>
       <c r="AF24" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AG24" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH24" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI24" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="AG24" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH24" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI24" t="s" s="2">
-        <v>199</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>99</v>
@@ -4077,10 +3943,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4189,10 +4055,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4303,10 +4169,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4419,10 +4285,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4448,13 +4314,13 @@
         <v>107</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4483,10 +4349,10 @@
         <v>127</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="Z28" t="s" s="2">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>77</v>
@@ -4504,7 +4370,7 @@
         <v>77</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>78</v>
@@ -4533,10 +4399,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4559,16 +4425,16 @@
         <v>88</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N29" t="s" s="2">
         <v>210</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -4618,7 +4484,7 @@
         <v>77</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>78</v>
@@ -4647,10 +4513,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4676,10 +4542,10 @@
         <v>145</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4730,16 +4596,16 @@
         <v>77</v>
       </c>
       <c r="AF30" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH30" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI30" t="s" s="2">
         <v>214</v>
-      </c>
-      <c r="AG30" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH30" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI30" t="s" s="2">
-        <v>217</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>99</v>
@@ -4759,10 +4625,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4871,10 +4737,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -4985,10 +4851,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5101,10 +4967,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5130,10 +4996,10 @@
         <v>107</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5163,10 +5029,10 @@
         <v>127</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Z34" t="s" s="2">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="AA34" t="s" s="2">
         <v>77</v>
@@ -5184,7 +5050,7 @@
         <v>77</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>87</v>
@@ -5213,10 +5079,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5242,13 +5108,13 @@
         <v>101</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5298,7 +5164,7 @@
         <v>77</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>87</v>
@@ -5327,10 +5193,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5356,10 +5222,10 @@
         <v>150</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -5410,7 +5276,7 @@
         <v>77</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>78</v>
@@ -5439,10 +5305,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5468,10 +5334,10 @@
         <v>132</v>
       </c>
       <c r="L37" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="M37" t="s" s="2">
         <v>231</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>234</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
@@ -5522,7 +5388,7 @@
         <v>77</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>78</v>
@@ -5551,10 +5417,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5580,10 +5446,10 @@
         <v>150</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
@@ -5634,7 +5500,7 @@
         <v>77</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>78</v>
@@ -5663,10 +5529,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5692,10 +5558,10 @@
         <v>150</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -5746,7 +5612,7 @@
         <v>77</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>78</v>
@@ -5775,10 +5641,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -5804,10 +5670,10 @@
         <v>145</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -5858,16 +5724,16 @@
         <v>77</v>
       </c>
       <c r="AF40" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI40" t="s" s="2">
         <v>241</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>244</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>99</v>
@@ -5887,10 +5753,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -5999,10 +5865,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6113,10 +5979,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6229,10 +6095,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6258,10 +6124,10 @@
         <v>150</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6312,7 +6178,7 @@
         <v>77</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>87</v>
@@ -6341,10 +6207,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6370,10 +6236,10 @@
         <v>101</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -6424,7 +6290,7 @@
         <v>77</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>78</v>
@@ -6453,10 +6319,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6482,13 +6348,13 @@
         <v>150</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -6538,7 +6404,7 @@
         <v>77</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>78</v>
@@ -6567,10 +6433,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6596,13 +6462,13 @@
         <v>132</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -6652,7 +6518,7 @@
         <v>77</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>78</v>
@@ -6681,10 +6547,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6707,16 +6573,16 @@
         <v>88</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -6766,7 +6632,7 @@
         <v>77</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
@@ -6795,23 +6661,21 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>175</v>
-      </c>
-      <c r="C49" t="s" s="2">
-        <v>267</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
         <v>77</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>77</v>
@@ -6823,16 +6687,20 @@
         <v>88</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>145</v>
+        <v>264</v>
       </c>
       <c r="L49" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="M49" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="O49" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="M49" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
       <c r="P49" t="s" s="2">
         <v>77</v>
       </c>
@@ -6880,19 +6748,19 @@
         <v>77</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>175</v>
+        <v>263</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>77</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>181</v>
+        <v>99</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>77</v>
@@ -6904,3634 +6772,6 @@
         <v>77</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B50" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E50" s="2"/>
-      <c r="F50" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G50" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K50" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q50" s="2"/>
-      <c r="R50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF50" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="AG50" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH50" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AK50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL50" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN50" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="B51" t="s" s="2">
-        <v>183</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="E51" s="2"/>
-      <c r="F51" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G51" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O51" s="2"/>
-      <c r="P51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q51" s="2"/>
-      <c r="R51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF51" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="AG51" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH51" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ51" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL51" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM51" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN51" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="B52" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="E52" s="2"/>
-      <c r="F52" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G52" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I52" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="J52" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K52" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O52" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="P52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q52" s="2"/>
-      <c r="R52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF52" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AG52" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH52" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ52" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN52" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="B53" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="C53" s="2"/>
-      <c r="D53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E53" s="2"/>
-      <c r="F53" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G53" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J53" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K53" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="M53" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q53" s="2"/>
-      <c r="R53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF53" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="AG53" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH53" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ53" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN53" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="B54" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="F54" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>190</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="O54" s="2"/>
-      <c r="P54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q54" s="2"/>
-      <c r="R54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN54" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="B55" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="C55" s="2"/>
-      <c r="D55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="G55" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="O55" s="2"/>
-      <c r="P55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q55" s="2"/>
-      <c r="R55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF55" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="AG55" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH55" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AK55" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="AN55" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="B56" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="C56" s="2"/>
-      <c r="D56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G56" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J56" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K56" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q56" s="2"/>
-      <c r="R56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="AG56" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH56" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI56" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="AJ56" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM56" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN56" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="B57" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="C57" s="2"/>
-      <c r="D57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E57" s="2"/>
-      <c r="F57" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G57" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K57" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
-      <c r="P57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q57" s="2"/>
-      <c r="R57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF57" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="AG57" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH57" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN57" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="B58" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="C58" s="2"/>
-      <c r="D58" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="E58" s="2"/>
-      <c r="F58" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G58" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K58" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O58" s="2"/>
-      <c r="P58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q58" s="2"/>
-      <c r="R58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF58" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="AG58" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH58" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ58" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL58" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN58" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="B59" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="C59" s="2"/>
-      <c r="D59" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="E59" s="2"/>
-      <c r="F59" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G59" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I59" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="J59" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K59" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O59" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="P59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q59" s="2"/>
-      <c r="R59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF59" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AG59" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH59" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ59" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL59" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM59" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN59" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s" s="2">
-        <v>285</v>
-      </c>
-      <c r="B60" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="C60" s="2"/>
-      <c r="D60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="F60" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G60" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J60" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K60" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="O60" s="2"/>
-      <c r="P60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q60" s="2"/>
-      <c r="R60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X60" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="Y60" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="Z60" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="AA60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF60" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="AG60" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH60" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ60" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM60" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN60" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="B61" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E61" s="2"/>
-      <c r="F61" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G61" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J61" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K61" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="L61" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="O61" s="2"/>
-      <c r="P61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q61" s="2"/>
-      <c r="R61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF61" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="AG61" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH61" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM61" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN61" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="B62" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="C62" s="2"/>
-      <c r="D62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="G62" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J62" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K62" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="L62" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q62" s="2"/>
-      <c r="R62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF62" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="AG62" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH62" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI62" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="AJ62" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM62" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="2">
-        <v>288</v>
-      </c>
-      <c r="B63" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E63" s="2"/>
-      <c r="F63" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G63" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K63" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q63" s="2"/>
-      <c r="R63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF63" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="AG63" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH63" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AK63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL63" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN63" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="2">
-        <v>289</v>
-      </c>
-      <c r="B64" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="E64" s="2"/>
-      <c r="F64" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G64" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K64" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O64" s="2"/>
-      <c r="P64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q64" s="2"/>
-      <c r="R64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF64" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="AG64" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH64" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ64" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL64" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN64" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="2">
-        <v>290</v>
-      </c>
-      <c r="B65" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="C65" s="2"/>
-      <c r="D65" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="E65" s="2"/>
-      <c r="F65" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G65" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I65" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="J65" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K65" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O65" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="P65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q65" s="2"/>
-      <c r="R65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF65" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AG65" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH65" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ65" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL65" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM65" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN65" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="2">
-        <v>291</v>
-      </c>
-      <c r="B66" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="C66" s="2"/>
-      <c r="D66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E66" s="2"/>
-      <c r="F66" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="G66" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J66" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K66" t="s" s="2">
-        <v>107</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2"/>
-      <c r="P66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q66" s="2"/>
-      <c r="R66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S66" t="s" s="2">
-        <v>292</v>
-      </c>
-      <c r="T66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X66" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="Y66" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="Z66" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="AA66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF66" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="AG66" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AH66" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ66" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM66" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN66" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="2">
-        <v>293</v>
-      </c>
-      <c r="B67" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E67" s="2"/>
-      <c r="F67" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="G67" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J67" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K67" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="L67" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="N67" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="O67" s="2"/>
-      <c r="P67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q67" s="2"/>
-      <c r="R67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF67" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="AG67" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AH67" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ67" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM67" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN67" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G68" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J68" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K68" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-      <c r="P68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q68" s="2"/>
-      <c r="R68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF68" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="AG68" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH68" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ68" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM68" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN68" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="B69" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="C69" s="2"/>
-      <c r="D69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E69" s="2"/>
-      <c r="F69" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G69" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J69" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K69" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="L69" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M69" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2"/>
-      <c r="P69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q69" s="2"/>
-      <c r="R69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF69" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ69" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM69" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN69" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="2">
-        <v>296</v>
-      </c>
-      <c r="B70" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="C70" s="2"/>
-      <c r="D70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E70" s="2"/>
-      <c r="F70" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G70" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J70" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K70" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="M70" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="N70" s="2"/>
-      <c r="O70" s="2"/>
-      <c r="P70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q70" s="2"/>
-      <c r="R70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF70" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="AG70" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH70" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ70" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM70" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN70" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s" s="2">
-        <v>297</v>
-      </c>
-      <c r="B71" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E71" s="2"/>
-      <c r="F71" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G71" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J71" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K71" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-      <c r="P71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q71" s="2"/>
-      <c r="R71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF71" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="AG71" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH71" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ71" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM71" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN71" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="B72" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E72" s="2"/>
-      <c r="F72" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G72" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J72" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K72" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="L72" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="N72" s="2"/>
-      <c r="O72" s="2"/>
-      <c r="P72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q72" s="2"/>
-      <c r="R72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF72" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="AG72" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH72" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI72" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM72" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN72" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="B73" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="C73" s="2"/>
-      <c r="D73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E73" s="2"/>
-      <c r="F73" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G73" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K73" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L73" t="s" s="2">
-        <v>151</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="N73" s="2"/>
-      <c r="O73" s="2"/>
-      <c r="P73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q73" s="2"/>
-      <c r="R73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF73" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AK73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL73" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN73" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="B74" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="C74" s="2"/>
-      <c r="D74" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G74" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="K74" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L74" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="M74" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O74" s="2"/>
-      <c r="P74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q74" s="2"/>
-      <c r="R74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL74" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN74" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="2">
-        <v>301</v>
-      </c>
-      <c r="B75" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="C75" s="2"/>
-      <c r="D75" t="s" s="2">
-        <v>164</v>
-      </c>
-      <c r="E75" s="2"/>
-      <c r="F75" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G75" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="H75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I75" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="J75" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K75" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="N75" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="O75" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="P75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q75" s="2"/>
-      <c r="R75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF75" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="AG75" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH75" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="AI75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL75" t="s" s="2">
-        <v>84</v>
-      </c>
-      <c r="AM75" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN75" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s" s="2">
-        <v>302</v>
-      </c>
-      <c r="B76" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="C76" s="2"/>
-      <c r="D76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E76" s="2"/>
-      <c r="F76" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="G76" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J76" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K76" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L76" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="M76" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="N76" s="2"/>
-      <c r="O76" s="2"/>
-      <c r="P76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q76" s="2"/>
-      <c r="R76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF76" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="AG76" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AH76" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ76" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN76" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="B77" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="C77" s="2"/>
-      <c r="D77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E77" s="2"/>
-      <c r="F77" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G77" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J77" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K77" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="L77" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="N77" s="2"/>
-      <c r="O77" s="2"/>
-      <c r="P77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q77" s="2"/>
-      <c r="R77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF77" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="AG77" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH77" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ77" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN77" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="B78" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="C78" s="2"/>
-      <c r="D78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E78" s="2"/>
-      <c r="F78" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G78" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J78" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K78" t="s" s="2">
-        <v>150</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="N78" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="O78" s="2"/>
-      <c r="P78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q78" s="2"/>
-      <c r="R78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF78" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="AG78" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH78" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ78" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM78" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN78" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="B79" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E79" s="2"/>
-      <c r="F79" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G79" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J79" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K79" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="L79" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="M79" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="N79" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="O79" s="2"/>
-      <c r="P79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q79" s="2"/>
-      <c r="R79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF79" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="AG79" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH79" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ79" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM79" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN79" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s" s="2">
-        <v>306</v>
-      </c>
-      <c r="B80" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="C80" s="2"/>
-      <c r="D80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E80" s="2"/>
-      <c r="F80" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G80" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J80" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K80" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="L80" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="M80" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="O80" s="2"/>
-      <c r="P80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q80" s="2"/>
-      <c r="R80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF80" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="AG80" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH80" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AK80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM80" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN80" t="s" s="2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="B81" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="C81" s="2"/>
-      <c r="D81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="E81" s="2"/>
-      <c r="F81" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="G81" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="H81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="I81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="J81" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="K81" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="L81" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="M81" t="s" s="2">
-        <v>310</v>
-      </c>
-      <c r="N81" t="s" s="2">
-        <v>311</v>
-      </c>
-      <c r="O81" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="P81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Q81" s="2"/>
-      <c r="R81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="S81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="T81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="U81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="V81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="W81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="X81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Y81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="Z81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AA81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AB81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AC81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AD81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AE81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AF81" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="AG81" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH81" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AJ81" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="AK81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AL81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM81" t="s" s="2">
-        <v>77</v>
-      </c>
-      <c r="AN81" t="s" s="2">
         <v>77</v>
       </c>
     </row>

</xml_diff>